<commit_message>
refactor: reorganize configuration and improve Chrome driver setup
</commit_message>
<xml_diff>
--- a/Planilhas/planilha_teste.xlsx
+++ b/Planilhas/planilha_teste.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">PDV</t>
   </si>
@@ -59,25 +59,10 @@
     <t xml:space="preserve">ARRUMAR</t>
   </si>
   <si>
-    <t xml:space="preserve">Alice</t>
+    <t xml:space="preserve">João</t>
   </si>
   <si>
     <t xml:space="preserve">Não recebimento de entrega</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gabriel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cauã</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leonardo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Miguel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">João</t>
   </si>
 </sst>
 </file>
@@ -494,7 +479,7 @@
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
     <cellStyle name="Excel Built-in Bad" xfId="20"/>
   </cellStyles>
-  <dxfs count="50">
+  <dxfs count="21">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -608,147 +593,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C5700"/>
       </font>
@@ -780,16 +624,6 @@
       <font>
         <color rgb="FF9C0006"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
     </dxf>
     <dxf>
       <fill>
@@ -809,127 +643,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -2714,8 +2427,8 @@
   </sheetPr>
   <dimension ref="A1:K157"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2770,141 +2483,56 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="13" t="n">
-        <v>19996389319</v>
-      </c>
+      <c r="A2" s="8"/>
+      <c r="C2" s="13"/>
       <c r="D2" s="14"/>
-      <c r="E2" s="15" t="n">
-        <v>45955</v>
-      </c>
-      <c r="F2" s="9" t="n">
-        <v>45955</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>12</v>
-      </c>
+      <c r="E2" s="15"/>
+      <c r="H2" s="16"/>
       <c r="J2" s="17"/>
-      <c r="K2" s="7" t="str">
-        <f aca="false">TRIM(UPPER(Tabela3[[#This Row],[MOTORISTA]]))</f>
-        <v/>
-      </c>
+      <c r="K2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="18" t="n">
-        <v>19989825908</v>
-      </c>
+      <c r="A3" s="8"/>
+      <c r="C3" s="18"/>
       <c r="D3" s="19"/>
-      <c r="E3" s="15" t="n">
-        <v>45956</v>
-      </c>
-      <c r="F3" s="9" t="n">
-        <v>45956</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>12</v>
-      </c>
+      <c r="E3" s="15"/>
+      <c r="H3" s="16"/>
       <c r="J3" s="17"/>
-      <c r="K3" s="7" t="str">
-        <f aca="false">TRIM(UPPER(Tabela3[[#This Row],[MOTORISTA]]))</f>
-        <v/>
-      </c>
+      <c r="K3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="18" t="n">
-        <v>19989177073</v>
-      </c>
+      <c r="A4" s="8"/>
+      <c r="C4" s="18"/>
       <c r="D4" s="14"/>
-      <c r="E4" s="15" t="n">
-        <v>45957</v>
-      </c>
-      <c r="F4" s="9" t="n">
-        <v>45957</v>
-      </c>
-      <c r="H4" s="16" t="s">
-        <v>12</v>
-      </c>
+      <c r="E4" s="15"/>
+      <c r="H4" s="16"/>
       <c r="J4" s="17"/>
-      <c r="K4" s="7" t="str">
-        <f aca="false">TRIM(UPPER(Tabela3[[#This Row],[MOTORISTA]]))</f>
-        <v/>
-      </c>
+      <c r="K4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="18" t="n">
-        <v>19997516604</v>
-      </c>
+      <c r="A5" s="8"/>
+      <c r="C5" s="18"/>
       <c r="D5" s="19"/>
-      <c r="E5" s="15" t="n">
-        <v>45958</v>
-      </c>
-      <c r="F5" s="9" t="n">
-        <v>45958</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>12</v>
-      </c>
+      <c r="E5" s="15"/>
+      <c r="H5" s="16"/>
       <c r="J5" s="17"/>
-      <c r="K5" s="7" t="str">
-        <f aca="false">TRIM(UPPER(Tabela3[[#This Row],[MOTORISTA]]))</f>
-        <v/>
-      </c>
+      <c r="K5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="18" t="n">
-        <v>19982272981</v>
-      </c>
+      <c r="A6" s="8"/>
+      <c r="C6" s="18"/>
       <c r="D6" s="19"/>
-      <c r="E6" s="15" t="n">
-        <v>45959</v>
-      </c>
-      <c r="F6" s="9" t="n">
-        <v>45959</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>12</v>
-      </c>
+      <c r="E6" s="15"/>
+      <c r="H6" s="16"/>
       <c r="J6" s="17"/>
-      <c r="K6" s="7" t="str">
-        <f aca="false">TRIM(UPPER(Tabela3[[#This Row],[MOTORISTA]]))</f>
-        <v/>
-      </c>
+      <c r="K6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C7" s="18" t="n">
         <v>19992558897</v>
@@ -4354,21 +3982,21 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G113">
+  <conditionalFormatting sqref="G113 G112 G110 G109 G103:G108 G148:G149 G154:G1048576 G1:G144">
     <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="STATUS" dxfId="7">
-      <formula>NOT(ISERROR(SEARCH("STATUS",G113)))</formula>
+      <formula>NOT(ISERROR(SEARCH("STATUS",G1)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="PENDENTE " dxfId="8">
-      <formula>NOT(ISERROR(SEARCH("PENDENTE ",G113)))</formula>
+      <formula>NOT(ISERROR(SEARCH("PENDENTE ",G1)))</formula>
     </cfRule>
     <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>"PENDENTE "</formula>
     </cfRule>
     <cfRule type="containsText" priority="5" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="STATUS" dxfId="10">
-      <formula>NOT(ISERROR(SEARCH("STATUS",G113)))</formula>
+      <formula>NOT(ISERROR(SEARCH("STATUS",G1)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="6" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="STATUS" dxfId="11">
-      <formula>NOT(ISERROR(SEARCH("STATUS",G113)))</formula>
+      <formula>NOT(ISERROR(SEARCH("STATUS",G1)))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="7">
       <colorScale>
@@ -4389,215 +4017,30 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G112">
-    <cfRule type="containsText" priority="9" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="STATUS" dxfId="12">
-      <formula>NOT(ISERROR(SEARCH("STATUS",G112)))</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="10" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="PENDENTE " dxfId="13">
-      <formula>NOT(ISERROR(SEARCH("PENDENTE ",G112)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="11" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
-      <formula>"PENDENTE "</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="12" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="STATUS" dxfId="15">
-      <formula>NOT(ISERROR(SEARCH("STATUS",G112)))</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="13" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="STATUS" dxfId="16">
-      <formula>NOT(ISERROR(SEARCH("STATUS",G112)))</formula>
-    </cfRule>
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEF9C"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G110">
-    <cfRule type="containsText" priority="16" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="STATUS" dxfId="17">
-      <formula>NOT(ISERROR(SEARCH("STATUS",G110)))</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="17" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="PENDENTE " dxfId="18">
-      <formula>NOT(ISERROR(SEARCH("PENDENTE ",G110)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="18" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
-      <formula>"PENDENTE "</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="19" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="STATUS" dxfId="20">
-      <formula>NOT(ISERROR(SEARCH("STATUS",G110)))</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="20" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="STATUS" dxfId="21">
-      <formula>NOT(ISERROR(SEARCH("STATUS",G110)))</formula>
-    </cfRule>
-    <cfRule type="colorScale" priority="21">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="22">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEF9C"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G109">
-    <cfRule type="containsText" priority="23" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="STATUS" dxfId="22">
-      <formula>NOT(ISERROR(SEARCH("STATUS",G109)))</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="24" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="PENDENTE " dxfId="23">
-      <formula>NOT(ISERROR(SEARCH("PENDENTE ",G109)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="25" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24">
-      <formula>"PENDENTE "</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="26" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="STATUS" dxfId="25">
-      <formula>NOT(ISERROR(SEARCH("STATUS",G109)))</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="27" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="STATUS" dxfId="26">
-      <formula>NOT(ISERROR(SEARCH("STATUS",G109)))</formula>
-    </cfRule>
-    <cfRule type="colorScale" priority="28">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="29">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEF9C"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C108 C104:C105">
-    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27"/>
+  <conditionalFormatting sqref="C108 C104:C105 C148:C149 C155 C122 C65 C49 C1 C9:C10 C34 C38:C39 C43 C69 C71:C72 C75 C77:C79 C83 C85:C86 C94:C96 C102 C124 C157:C1048576 B2:B157">
+    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2">
-    <cfRule type="containsText" priority="31" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="AGUARDANDO" dxfId="28">
+    <cfRule type="containsText" priority="10" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="AGUARDANDO" dxfId="13">
       <formula>NOT(ISERROR(SEARCH("AGUARDANDO",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G157">
-    <cfRule type="containsText" priority="32" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONCLUIDO" dxfId="29">
+    <cfRule type="containsText" priority="11" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONCLUIDO" dxfId="14">
       <formula>NOT(ISERROR(SEARCH("CONCLUIDO",G1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="top10" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="10" text="" dxfId="30"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C148:C149 C155 C122 C65 C49 C1 C9:C10 C34 C38:C39 C43 C69 C71:C72 C75 C77:C79 C83 C85:C86 C94:C96 C102 C124 C157:C1048576">
-    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31"/>
+    <cfRule type="top10" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="10" text="" dxfId="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2 D4">
-    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32"/>
-    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33"/>
-    <cfRule type="duplicateValues" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34"/>
+    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
+    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
+    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G103:G108">
-    <cfRule type="containsText" priority="38" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="STATUS" dxfId="35">
-      <formula>NOT(ISERROR(SEARCH("STATUS",G103)))</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="39" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="PENDENTE " dxfId="36">
-      <formula>NOT(ISERROR(SEARCH("PENDENTE ",G103)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="40" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37">
-      <formula>"PENDENTE "</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="41" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="STATUS" dxfId="38">
-      <formula>NOT(ISERROR(SEARCH("STATUS",G103)))</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="42" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="STATUS" dxfId="39">
-      <formula>NOT(ISERROR(SEARCH("STATUS",G103)))</formula>
-    </cfRule>
-    <cfRule type="colorScale" priority="43">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="44">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEF9C"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A103:A108">
-    <cfRule type="duplicateValues" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40"/>
-    <cfRule type="duplicateValues" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G148:G149 G154:G1048576 G1:G144">
-    <cfRule type="containsText" priority="47" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="STATUS" dxfId="42">
-      <formula>NOT(ISERROR(SEARCH("STATUS",G1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="48" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="PENDENTE " dxfId="43">
-      <formula>NOT(ISERROR(SEARCH("PENDENTE ",G1)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="49" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44">
-      <formula>"PENDENTE "</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="50" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="STATUS" dxfId="45">
-      <formula>NOT(ISERROR(SEARCH("STATUS",G1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="51" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="STATUS" dxfId="46">
-      <formula>NOT(ISERROR(SEARCH("STATUS",G1)))</formula>
-    </cfRule>
-    <cfRule type="colorScale" priority="52">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="53">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEF9C"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A148:A149 A154:A1048576 A109:A144 A1:A98 A102">
-    <cfRule type="duplicateValues" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47"/>
-    <cfRule type="duplicateValues" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B157">
-    <cfRule type="duplicateValues" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49"/>
+  <conditionalFormatting sqref="A103:A108 A148:A149 A154:A1048576 A109:A144 A1:A98 A102">
+    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
+    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>